<commit_message>
quitar "empleado de" y solo dejar la entidad
</commit_message>
<xml_diff>
--- a/HT-6/BAC-22-Catálogo de acciones estratégicas.xlsx
+++ b/HT-6/BAC-22-Catálogo de acciones estratégicas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB927B5-4140-F544-9F20-F2D9CE3B7280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D81500D-3982-4E45-9342-3AFBCF14C77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="36180" yWindow="-5560" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-22" sheetId="1" r:id="rId1"/>
@@ -156,19 +156,19 @@
     <t>Contratación de asesoría de imagen para la marca</t>
   </si>
   <si>
-    <t>Empleado de recursos humanos</t>
-  </si>
-  <si>
-    <t>Empleado asesor comercial</t>
-  </si>
-  <si>
-    <t>Empleado director logístico</t>
-  </si>
-  <si>
-    <t>Empleado asesor de imagen de marca</t>
-  </si>
-  <si>
     <t>Agencia publicitaria</t>
+  </si>
+  <si>
+    <t>Recursos humanos</t>
+  </si>
+  <si>
+    <t>Asesor comercial</t>
+  </si>
+  <si>
+    <t>Director logístico</t>
+  </si>
+  <si>
+    <t>Asesor de imagen de marca</t>
   </si>
 </sst>
 </file>
@@ -292,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -305,6 +305,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -317,34 +320,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +661,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+      <selection activeCell="D35" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -697,18 +696,18 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
@@ -737,431 +736,477 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="9"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="9"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="9"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="9"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="9"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="9"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="9"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="9"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="9"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="9"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="9"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="9"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-    </row>
-    <row r="37" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="15"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-    </row>
-    <row r="38" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="15"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="C15:C16"/>
@@ -1174,72 +1219,26 @@
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hay que esperar a que jorge responda
</commit_message>
<xml_diff>
--- a/HT-6/BAC-22-Catálogo de acciones estratégicas.xlsx
+++ b/HT-6/BAC-22-Catálogo de acciones estratégicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D81500D-3982-4E45-9342-3AFBCF14C77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863D3EB4-994B-F945-B389-8068EC2D3B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36180" yWindow="-5560" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Asesor de imagen de marca</t>
+  </si>
+  <si>
+    <t>Periódico cada 6 meses</t>
+  </si>
+  <si>
+    <t>Periódico cada año</t>
+  </si>
+  <si>
+    <t>Periódico cada 3 meses</t>
   </si>
 </sst>
 </file>
@@ -215,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -288,11 +297,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +361,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -315,15 +377,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -332,17 +397,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,7 +729,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:D36"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -696,18 +764,18 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="14"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
@@ -736,411 +804,516 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="20"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="20"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="10"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="20"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="10"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="20"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="20"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="10"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="23">
+        <v>45292</v>
+      </c>
+      <c r="F17" s="10"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="23">
+        <v>45352</v>
+      </c>
+      <c r="F21" s="23">
+        <v>45444</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="23">
+        <v>45566</v>
+      </c>
+      <c r="F23" s="23">
+        <v>45658</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="10"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="20"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="10"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="20"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="10"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="20"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="10"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="20"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="10"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7" t="s">
+      <c r="C33" s="10"/>
+      <c r="D33" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="10"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35" s="17"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="17"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38" s="17"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="98">
+  <mergeCells count="89">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:F26"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="E31:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="F35:F36"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:B38"/>
@@ -1153,92 +1326,6 @@
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambios muy necesarios en la estructura del negocio
</commit_message>
<xml_diff>
--- a/HT-6/BAC-22-Catálogo de acciones estratégicas.xlsx
+++ b/HT-6/BAC-22-Catálogo de acciones estratégicas.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD75AD4E-C6A4-D548-BA68-0D16B94A551C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA36729-5C22-6345-A49A-B1223EFBC7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36180" yWindow="-5560" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-22" sheetId="1" r:id="rId1"/>
+    <sheet name="Montar un local" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -78,12 +79,6 @@
     <t>AE-2</t>
   </si>
   <si>
-    <t>AE-3</t>
-  </si>
-  <si>
-    <t>AE-4</t>
-  </si>
-  <si>
     <t>AE-5</t>
   </si>
   <si>
@@ -93,21 +88,9 @@
     <t>AE-7</t>
   </si>
   <si>
-    <t>AE-8</t>
-  </si>
-  <si>
     <t>AE-9</t>
   </si>
   <si>
-    <t>AE-10</t>
-  </si>
-  <si>
-    <t>AE-11</t>
-  </si>
-  <si>
-    <t>AE-12</t>
-  </si>
-  <si>
     <t>AE-13</t>
   </si>
   <si>
@@ -165,21 +148,9 @@
     <t>Asesor comercial</t>
   </si>
   <si>
-    <t>Director logístico</t>
-  </si>
-  <si>
     <t>Asesor de imagen de marca</t>
   </si>
   <si>
-    <t>Periódico cada 6 meses</t>
-  </si>
-  <si>
-    <t>Periódico cada año</t>
-  </si>
-  <si>
-    <t>Periódico cada 3 meses</t>
-  </si>
-  <si>
     <t>AE-15</t>
   </si>
   <si>
@@ -190,6 +161,15 @@
   </si>
   <si>
     <t>Despliegue de marketplace fácilmente escalable</t>
+  </si>
+  <si>
+    <t>Instalación de nuevo punto de venta</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>Agencia de software</t>
   </si>
 </sst>
 </file>
@@ -222,7 +202,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,8 +215,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -309,55 +295,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -376,6 +318,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -383,22 +334,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -406,20 +351,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:H38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="111" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -746,7 +706,7 @@
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" customWidth="1"/>
     <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.83203125" customWidth="1"/>
     <col min="7" max="7" width="7.83203125" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
@@ -773,18 +733,18 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
@@ -813,467 +773,405 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="B7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="13"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="24"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="7"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
+    <row r="10" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>45</v>
-      </c>
+    <row r="11" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="13"/>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="7"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="13"/>
+    <row r="15" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="15">
+        <v>45292</v>
+      </c>
+      <c r="F15" s="9"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="7"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="19">
-        <v>45292</v>
-      </c>
-      <c r="F17" s="10"/>
+      <c r="A17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="7"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="A19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="15">
+        <v>45566</v>
+      </c>
+      <c r="F19" s="15">
+        <v>45658</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="19">
-        <v>45352</v>
-      </c>
-      <c r="F21" s="19">
-        <v>45444</v>
-      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="19">
-        <v>45566</v>
-      </c>
-      <c r="F23" s="19">
-        <v>45658</v>
-      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="13"/>
+      <c r="A25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="7"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10" t="s">
+      <c r="A27" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="13"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="7"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="7"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="13"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="7"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A34" s="7"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38" s="20"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-    </row>
+    <row r="33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="89">
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E25:F26"/>
-    <mergeCell ref="E27:F28"/>
+  <mergeCells count="78">
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="C31:C32"/>
@@ -1282,69 +1180,88 @@
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:F30"/>
-    <mergeCell ref="E31:F32"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F25:F26"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="E15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3D63CB-A623-BC49-B5CD-51A38787AAD6}">
+  <dimension ref="B4:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B4" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B6" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B7" s="16"/>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B8" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B10" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B12" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B14" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B15" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>